<commit_message>
Update Readme and testing Files
</commit_message>
<xml_diff>
--- a/assets/testing/GOLtesting.xlsx
+++ b/assets/testing/GOLtesting.xlsx
@@ -2893,7 +2893,7 @@
     </row>
     <row r="15" ht="80.35" customHeight="1">
       <c r="A15" s="9">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
       <c r="B15" t="s" s="10">
         <v>51</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="16" ht="80.35" customHeight="1">
       <c r="A16" s="9">
-        <v>7.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="B16" t="s" s="10">
         <v>55</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="17" ht="116.35" customHeight="1">
       <c r="A17" s="9">
-        <v>7.6</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="B17" t="s" s="10">
         <v>59</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="18" ht="68.35" customHeight="1">
       <c r="A18" s="9">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="B18" t="s" s="10">
         <v>63</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="19" ht="68.35" customHeight="1">
       <c r="A19" s="9">
-        <v>9.1</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="B19" t="s" s="10">
         <v>67</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="20" ht="68.35" customHeight="1">
       <c r="A20" s="9">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="B20" t="s" s="10">
         <v>71</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="21" ht="56.35" customHeight="1">
       <c r="A21" s="9">
-        <v>9.300000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="B21" t="s" s="10">
         <v>75</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="22" ht="68.35" customHeight="1">
       <c r="A22" s="9">
-        <v>9.4</v>
+        <v>9.5</v>
       </c>
       <c r="B22" t="s" s="10">
         <v>79</v>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="23" ht="92.35" customHeight="1">
       <c r="A23" s="9">
-        <v>9.5</v>
+        <v>9.6</v>
       </c>
       <c r="B23" t="s" s="10">
         <v>83</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="24" ht="152.35" customHeight="1">
       <c r="A24" s="9">
-        <v>9.6</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="B24" t="s" s="10">
         <v>87</v>

</xml_diff>